<commit_message>
Statusbericht bis auf Teambarometer und Risikoanalyse abgeschlossen
</commit_message>
<xml_diff>
--- a/20-11-23_Statusbericht/20-11-20_Gantt_Chart.xlsx
+++ b/20-11-23_Statusbericht/20-11-20_Gantt_Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\AAA_Studium_HAW_Mechatronik\WiSe20\Bachelorprojekt\bachelorprojekt2020\20-11-23_Statusbericht\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FBBA02C-3DE8-4AAB-A8FD-8F0A5ED25F69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F06B25-F01D-4A4F-9709-EBEDE0D8DCCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{905C64CD-B653-4290-BF74-D3CE989EBBEF}"/>
   </bookViews>
@@ -211,8 +211,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7459134" y="998483"/>
-          <a:ext cx="2185044" cy="831443"/>
+          <a:off x="7461228" y="998483"/>
+          <a:ext cx="2185044" cy="825163"/>
           <a:chOff x="7460495" y="998483"/>
           <a:chExt cx="2185044" cy="817836"/>
         </a:xfrm>
@@ -316,6 +316,128 @@
           <a:p>
             <a:pPr algn="l"/>
             <a:endParaRPr lang="de-DE" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1006928</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>86044</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>108858</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="6" name="Gruppieren 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5B853E9-5332-42F6-A691-480981A88B45}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="7102928" y="857251"/>
+          <a:ext cx="441924" cy="9787722"/>
+          <a:chOff x="6721928" y="367393"/>
+          <a:chExt cx="439830" cy="9837964"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="4" name="Gerader Verbinder 3">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{499B13D5-4481-42F1-8F6C-A346FE258B77}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6721928" y="367393"/>
+            <a:ext cx="0" cy="9837964"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent2"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent2"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent2"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="5" name="Textfeld 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C64C643-6964-48E1-88D2-4FE81963C399}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="5400000">
+            <a:off x="6368143" y="5470072"/>
+            <a:ext cx="1213089" cy="374141"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="de-DE" sz="1800" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Heute Line</a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -624,8 +746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7D7FA78-90B6-4B5B-A677-AB96A65F19BC}">
   <dimension ref="A1:AA53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I49" sqref="I49"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>